<commit_message>
Changes to user validation. Details are not working yet but will have to get them to work.
</commit_message>
<xml_diff>
--- a/Testing Scenarions Bookings.xlsx
+++ b/Testing Scenarions Bookings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>People</t>
   </si>
@@ -87,6 +87,24 @@
   </si>
   <si>
     <t>Reutrn the c</t>
+  </si>
+  <si>
+    <t>If user registers, then person is automatically created.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If a person has made a booking before and then registers? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">does user email exist in Person table? </t>
+  </si>
+  <si>
+    <t>if yes, then update user ID</t>
+  </si>
+  <si>
+    <t>if no then, create person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If user </t>
   </si>
 </sst>
 </file>
@@ -426,15 +444,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="22.140625" style="1" bestFit="1" customWidth="1"/>
@@ -442,201 +460,231 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>2</v>
+      <c r="A1" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B16" s="2">
         <v>0</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C16" s="2">
         <v>0</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
         <v>0</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B18" s="2">
         <v>0</v>
       </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="2"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C21" s="2"/>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B13:C26 B4:C10">
+  <conditionalFormatting sqref="B25:C38 B16:C22">
     <cfRule type="iconSet" priority="5">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -645,7 +693,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:C12">
+  <conditionalFormatting sqref="B24:C24">
     <cfRule type="iconSet" priority="7">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -654,7 +702,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:H7">
+  <conditionalFormatting sqref="H18:H19">
     <cfRule type="iconSet" priority="3">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -663,7 +711,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
+  <conditionalFormatting sqref="H16">
     <cfRule type="iconSet" priority="2">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -672,7 +720,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
+  <conditionalFormatting sqref="H17">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -682,10 +730,10 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E7" r:id="rId4"/>
+    <hyperlink ref="E18" r:id="rId1"/>
+    <hyperlink ref="E16" r:id="rId2"/>
+    <hyperlink ref="E17" r:id="rId3"/>
+    <hyperlink ref="E19" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>